<commit_message>
spreadsheet updated with test data
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Downloads\VSCodeProjects\deepwokenItemBot\DeepBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1FD96E-1E32-4539-95F9-047F8D855C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F27FF1-6A29-453C-9352-44A9275D5908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86F9E6BA-CED1-4B8E-A36C-94AEAC79A48C}"/>
   </bookViews>
@@ -33,6 +33,194 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
+  <si>
+    <t>item_name</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>rarity</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>VOI</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Formless Shard</t>
+  </si>
+  <si>
+    <t>Stiletto</t>
+  </si>
+  <si>
+    <t>Gilded Knife</t>
+  </si>
+  <si>
+    <t>Silver Dagger</t>
+  </si>
+  <si>
+    <t>Canor Fang</t>
+  </si>
+  <si>
+    <t>Fool's Tankard</t>
+  </si>
+  <si>
+    <t>Whaling Knife</t>
+  </si>
+  <si>
+    <t>Champion's Dagger</t>
+  </si>
+  <si>
+    <t>Central Dirk</t>
+  </si>
+  <si>
+    <t>Tanto</t>
+  </si>
+  <si>
+    <t>Sanguine Transfuser</t>
+  </si>
+  <si>
+    <t>Nemit's Sickle</t>
+  </si>
+  <si>
+    <t>Flareblood Kamas</t>
+  </si>
+  <si>
+    <t>The Flippers of Fate</t>
+  </si>
+  <si>
+    <t>Krulian Knife</t>
+  </si>
+  <si>
+    <t>Spectral Grasp</t>
+  </si>
+  <si>
+    <t>Moppet</t>
+  </si>
+  <si>
+    <t>Kyrsedge</t>
+  </si>
+  <si>
+    <t>Alloyed Whaling Knife</t>
+  </si>
+  <si>
+    <t>Alloyed Tanto</t>
+  </si>
+  <si>
+    <t>Big Brother</t>
+  </si>
+  <si>
+    <t>Cerulean Thread</t>
+  </si>
+  <si>
+    <t>The Golden Fool</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>legendary</t>
+  </si>
+  <si>
+    <t>Anklets of Alsin</t>
+  </si>
+  <si>
+    <t>Iron Cestus</t>
+  </si>
+  <si>
+    <t>Legion Cestus</t>
+  </si>
+  <si>
+    <t>Light's Final Toll</t>
+  </si>
+  <si>
+    <t>Wraithclaw</t>
+  </si>
+  <si>
+    <t>Coral Cestus</t>
+  </si>
+  <si>
+    <t>Flamekeeper Cestus</t>
+  </si>
+  <si>
+    <t>Vortex Echo</t>
+  </si>
+  <si>
+    <t>Drakemaw Gauntlets</t>
+  </si>
+  <si>
+    <t>Gaunts of Enmity</t>
+  </si>
+  <si>
+    <t>Broodalloy Cestus</t>
+  </si>
+  <si>
+    <t>Worldpiercer Gauntlets</t>
+  </si>
+  <si>
+    <t>Sovereign Bangle</t>
+  </si>
+  <si>
+    <t>The Death Knell</t>
+  </si>
+  <si>
+    <t>Frost Gauntlets</t>
+  </si>
+  <si>
+    <t>Quickfang</t>
+  </si>
+  <si>
+    <t>Apprentice Rapier</t>
+  </si>
+  <si>
+    <t>Inquisitor's Thorn</t>
+  </si>
+  <si>
+    <t>Deepspindle</t>
+  </si>
+  <si>
+    <t>Crucible Rapier</t>
+  </si>
+  <si>
+    <t>Golden Swordfish</t>
+  </si>
+  <si>
+    <t>Needle's Eye</t>
+  </si>
+  <si>
+    <t>Skull Piercer</t>
+  </si>
+  <si>
+    <t>Kyrstreza</t>
+  </si>
+  <si>
+    <t>Icepick</t>
+  </si>
+  <si>
+    <t>Light/dagger</t>
+  </si>
+  <si>
+    <t>Light/fist</t>
+  </si>
+  <si>
+    <t>relic</t>
+  </si>
+  <si>
+    <t>subcategories</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +254,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,14 +591,541 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BA666F-0039-44A8-827C-42AE5BC8B4DE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F63" s="1"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F65" s="1"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="1"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F72" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
items sheet updated for all weapons
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Downloads\VSCodeProjects\deepwokenItemBot\DeepBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC555886-20A4-4052-9A55-AEFE065AF43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C778929-2FA8-493F-8ADA-EE7981AB53A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{86F9E6BA-CED1-4B8E-A36C-94AEAC79A48C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86F9E6BA-CED1-4B8E-A36C-94AEAC79A48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="243">
   <si>
     <t>item_name</t>
   </si>
@@ -261,6 +261,510 @@
   </si>
   <si>
     <t>Medium/Sword</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>Dormant Splinter</t>
+  </si>
+  <si>
+    <t>Messer</t>
+  </si>
+  <si>
+    <t>Falchion</t>
+  </si>
+  <si>
+    <t>Scimitar</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
+  <si>
+    <t>Worshipper Longsword</t>
+  </si>
+  <si>
+    <t>Officer Saber</t>
+  </si>
+  <si>
+    <t>Vigil Longsword</t>
+  </si>
+  <si>
+    <t>Champion's Sword</t>
+  </si>
+  <si>
+    <t>Cavalry Saber</t>
+  </si>
+  <si>
+    <t>Curved Blade of Winds</t>
+  </si>
+  <si>
+    <t>Shotel</t>
+  </si>
+  <si>
+    <t>Warden Ceremonial Sword</t>
+  </si>
+  <si>
+    <t>Kindred Edict</t>
+  </si>
+  <si>
+    <t>Scoundrel's Saber</t>
+  </si>
+  <si>
+    <t>Razor Cutlass</t>
+  </si>
+  <si>
+    <t>Wyrmtooth</t>
+  </si>
+  <si>
+    <t>Forgotten Gladius</t>
+  </si>
+  <si>
+    <t>Fondant Splitter</t>
+  </si>
+  <si>
+    <t>Umbrite Witherblade</t>
+  </si>
+  <si>
+    <t>Serpent's Edge</t>
+  </si>
+  <si>
+    <t>Hallowscleave</t>
+  </si>
+  <si>
+    <t>Alloyed Messer</t>
+  </si>
+  <si>
+    <t>Alloyed Cavalry Saber</t>
+  </si>
+  <si>
+    <t>Alloyed Officer Saber</t>
+  </si>
+  <si>
+    <t>Alloyed Falchion</t>
+  </si>
+  <si>
+    <t>Alloyed Vigil Longsword</t>
+  </si>
+  <si>
+    <t>Alloyed Shotel</t>
+  </si>
+  <si>
+    <t>Alloyed Katana</t>
+  </si>
+  <si>
+    <t>Kyrsblade</t>
+  </si>
+  <si>
+    <t>Rite of Authority</t>
+  </si>
+  <si>
+    <t>Eye of Malice</t>
+  </si>
+  <si>
+    <t>Soulthorn</t>
+  </si>
+  <si>
+    <t>Purple Cloud</t>
+  </si>
+  <si>
+    <t>Shattered Katana</t>
+  </si>
+  <si>
+    <t>Nocturne</t>
+  </si>
+  <si>
+    <t>Hero's Blade of Flame</t>
+  </si>
+  <si>
+    <t>Hero's Blade of Frost</t>
+  </si>
+  <si>
+    <t>Hero's Blade of Lightning</t>
+  </si>
+  <si>
+    <t>Hero's Blade of Wind</t>
+  </si>
+  <si>
+    <t>Hero's Blade of Shadow</t>
+  </si>
+  <si>
+    <t>Ferractine</t>
+  </si>
+  <si>
+    <t>Phantomcleave</t>
+  </si>
+  <si>
+    <t>Ignition Deepcrusher</t>
+  </si>
+  <si>
+    <t>Medium/Heavy/Sword/Hybrid</t>
+  </si>
+  <si>
+    <t>Medium/Sword/hallowtide</t>
+  </si>
+  <si>
+    <t>Medium/Sword/Elemental/Flame</t>
+  </si>
+  <si>
+    <t>Medium/Sword/Elemental/Thunder</t>
+  </si>
+  <si>
+    <t>Medium/Sword/Elemental/Frost</t>
+  </si>
+  <si>
+    <t>Medium/Sword/Elemental/Gale</t>
+  </si>
+  <si>
+    <t>Medium/Sword/Elemental/Shadow</t>
+  </si>
+  <si>
+    <t>Light/dagger/Elemental/Blood</t>
+  </si>
+  <si>
+    <t>Light/fist/Elemental/Gale</t>
+  </si>
+  <si>
+    <t>Light/Pistol/Elemental/Iron</t>
+  </si>
+  <si>
+    <t>Light/Rapier/Elemental/Shadow</t>
+  </si>
+  <si>
+    <t>Medium/Sword/Club/Elemental/Iron</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Pleeksty's Inferno</t>
+  </si>
+  <si>
+    <t>Sacred Hammer</t>
+  </si>
+  <si>
+    <t>The Pastry Paster</t>
+  </si>
+  <si>
+    <t>Toothed Club </t>
+  </si>
+  <si>
+    <t>Morning Star </t>
+  </si>
+  <si>
+    <t>Pernach </t>
+  </si>
+  <si>
+    <t>Night Star </t>
+  </si>
+  <si>
+    <t>Medium/Club</t>
+  </si>
+  <si>
+    <t>Medium/Club/Elemental/Flame</t>
+  </si>
+  <si>
+    <t>Medium/Spear</t>
+  </si>
+  <si>
+    <t>Iron Spear</t>
+  </si>
+  <si>
+    <t>Gremorian Longspear</t>
+  </si>
+  <si>
+    <t>Ritual Spear</t>
+  </si>
+  <si>
+    <t>Ritual Sacrifice</t>
+  </si>
+  <si>
+    <t>Imperial Staff</t>
+  </si>
+  <si>
+    <t>Red Death (Bleed)</t>
+  </si>
+  <si>
+    <t>Trident Spear</t>
+  </si>
+  <si>
+    <t>The Weaving Web</t>
+  </si>
+  <si>
+    <t>Alloyed Longspear</t>
+  </si>
+  <si>
+    <t>Rifle Spear</t>
+  </si>
+  <si>
+    <t>True Seraph's Spear</t>
+  </si>
+  <si>
+    <t>Weal and Woe</t>
+  </si>
+  <si>
+    <t>Imperator's Edge</t>
+  </si>
+  <si>
+    <t>Alloyed Trident Spear</t>
+  </si>
+  <si>
+    <t>Kyrsglaive (Bleed)</t>
+  </si>
+  <si>
+    <t>Acheron's Warspear </t>
+  </si>
+  <si>
+    <t>Medium/Spear/Hybrid</t>
+  </si>
+  <si>
+    <t>Kyrswynter </t>
+  </si>
+  <si>
+    <t>Medium/Spear/Elemental/Frost</t>
+  </si>
+  <si>
+    <t>Medium/Spear/Hallowtide</t>
+  </si>
+  <si>
+    <t>Serrated Warspear</t>
+  </si>
+  <si>
+    <t>Bloodtide Trident </t>
+  </si>
+  <si>
+    <t>Medium/Spear/Elemental/Shadow</t>
+  </si>
+  <si>
+    <t>Medium/Spear/Elemental/Blood/Shadow</t>
+  </si>
+  <si>
+    <t>Medium/Rifle</t>
+  </si>
+  <si>
+    <t>Summer Rifle</t>
+  </si>
+  <si>
+    <t>Rosen's Hellflame</t>
+  </si>
+  <si>
+    <t>Stormseye</t>
+  </si>
+  <si>
+    <t>Rosen's Peacemaker</t>
+  </si>
+  <si>
+    <t>Iron Blunderbuss</t>
+  </si>
+  <si>
+    <t>Winter Rifle</t>
+  </si>
+  <si>
+    <t>Vapormaw Carbine</t>
+  </si>
+  <si>
+    <t>Medium/Rifle/Elemental/Flame</t>
+  </si>
+  <si>
+    <t>Medium/Rifle/Elemental/Thunder</t>
+  </si>
+  <si>
+    <t>Iron Twinblade</t>
+  </si>
+  <si>
+    <t>Scalesplitter</t>
+  </si>
+  <si>
+    <t>Alloyed Scalesplitter</t>
+  </si>
+  <si>
+    <t>Crescendo</t>
+  </si>
+  <si>
+    <t>Depthsplitter</t>
+  </si>
+  <si>
+    <t>Medium/Twinblade</t>
+  </si>
+  <si>
+    <t>Medium/Twinblade/Hallowtide</t>
+  </si>
+  <si>
+    <t>Death's Reverie 7</t>
+  </si>
+  <si>
+    <t>Guiding Star</t>
+  </si>
+  <si>
+    <t>Medium/Bow</t>
+  </si>
+  <si>
+    <t>Battleaxe</t>
+  </si>
+  <si>
+    <t>Halberd</t>
+  </si>
+  <si>
+    <t>Adretian Axe</t>
+  </si>
+  <si>
+    <t>Canorian Axe</t>
+  </si>
+  <si>
+    <t>Gran Sudaruska</t>
+  </si>
+  <si>
+    <t>Iron Birch</t>
+  </si>
+  <si>
+    <t>Master Hawk's Handaxe</t>
+  </si>
+  <si>
+    <t>Relic Axe</t>
+  </si>
+  <si>
+    <t>Quartztone Pickaxe</t>
+  </si>
+  <si>
+    <t>Skyreap Blade</t>
+  </si>
+  <si>
+    <t>Enforcer's Axe</t>
+  </si>
+  <si>
+    <t>Alloyed Canorian Axe</t>
+  </si>
+  <si>
+    <t>Alloyed Halberd</t>
+  </si>
+  <si>
+    <t>Alloyed Adretian Axe</t>
+  </si>
+  <si>
+    <t>Duskguard Axe</t>
+  </si>
+  <si>
+    <t>Night Axe</t>
+  </si>
+  <si>
+    <t>Pale Briar</t>
+  </si>
+  <si>
+    <t>Chorus of Agonies</t>
+  </si>
+  <si>
+    <t>Par's Glaive</t>
+  </si>
+  <si>
+    <t>Heavy/Greataxe</t>
+  </si>
+  <si>
+    <t>Heavy/Greataxe/Elemental/Frost</t>
+  </si>
+  <si>
+    <t>Evanspear Greataxe </t>
+  </si>
+  <si>
+    <t>Heavy/Greataxe/Hallowtide</t>
+  </si>
+  <si>
+    <t>Heavy/Greatsword</t>
+  </si>
+  <si>
+    <t>Zweihander</t>
+  </si>
+  <si>
+    <t>Ysley's Pyre Keeper</t>
+  </si>
+  <si>
+    <t>Markor's Inheritor</t>
+  </si>
+  <si>
+    <t>Darksteel Greatsword</t>
+  </si>
+  <si>
+    <t>Inquisitor's Greatsword</t>
+  </si>
+  <si>
+    <t>Crypt Blade</t>
+  </si>
+  <si>
+    <t>Kyrsieger</t>
+  </si>
+  <si>
+    <t>Bloodbane</t>
+  </si>
+  <si>
+    <t>Hailbreaker</t>
+  </si>
+  <si>
+    <t>Wretched Mawblades</t>
+  </si>
+  <si>
+    <t>First Light</t>
+  </si>
+  <si>
+    <t>Alloyed Zweihander</t>
+  </si>
+  <si>
+    <t>Darkalloy Greatsword</t>
+  </si>
+  <si>
+    <t>Alloyed Inheritor</t>
+  </si>
+  <si>
+    <t>Railblade</t>
+  </si>
+  <si>
+    <t>Enforcer's Blade</t>
+  </si>
+  <si>
+    <t>Metal Greatsword</t>
+  </si>
+  <si>
+    <t>Soulwrought Greatsword</t>
+  </si>
+  <si>
+    <t>Prototype Railblade</t>
+  </si>
+  <si>
+    <t>Darksteel Cleaver</t>
+  </si>
+  <si>
+    <t>Crescent Cleaver (Bleed)</t>
+  </si>
+  <si>
+    <t>Bloodfouler (Bleed)</t>
+  </si>
+  <si>
+    <t>The Long Tong of The Law (Bleed)</t>
+  </si>
+  <si>
+    <t>Alloyed Crescent Cleaver (Bleed)</t>
+  </si>
+  <si>
+    <t>Kyrscleave (Bleed)</t>
+  </si>
+  <si>
+    <t>Fractine (Bleed)(BRKN)</t>
+  </si>
+  <si>
+    <t>Lumensplitter (Bleed)</t>
+  </si>
+  <si>
+    <t>Heavy/Greatsword/Hybrid</t>
+  </si>
+  <si>
+    <t>Heavy/Greatsword/Hybrid/Elemental/Flame</t>
+  </si>
+  <si>
+    <t>named</t>
+  </si>
+  <si>
+    <t>Heavy/Greatsword/Elemental/Blood</t>
+  </si>
+  <si>
+    <t>Heavy/Greatsword/Elemental/Shadow</t>
   </si>
 </sst>
 </file>
@@ -633,17 +1137,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BA666F-0039-44A8-827C-42AE5BC8B4DE}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I54" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
@@ -790,7 +1294,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
         <v>58</v>
@@ -982,7 +1486,7 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
         <v>31</v>
@@ -1136,7 +1640,7 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="D46" t="s">
         <v>31</v>
@@ -1255,7 +1759,7 @@
         <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="D56" t="s">
         <v>31</v>
@@ -1323,6 +1827,9 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>75</v>
+      </c>
       <c r="C62" t="s">
         <v>74</v>
       </c>
@@ -1331,33 +1838,1507 @@
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
       <c r="D63" t="s">
         <v>58</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>74</v>
+      </c>
       <c r="D64" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" t="s">
+        <v>30</v>
+      </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" t="s">
+        <v>30</v>
+      </c>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" t="s">
+        <v>30</v>
+      </c>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" t="s">
+        <v>30</v>
+      </c>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" t="s">
+        <v>30</v>
+      </c>
       <c r="F70" s="1"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" t="s">
+        <v>30</v>
+      </c>
       <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" t="s">
+        <v>74</v>
+      </c>
+      <c r="D79" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>93</v>
+      </c>
+      <c r="C81" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" t="s">
+        <v>30</v>
+      </c>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" t="s">
+        <v>74</v>
+      </c>
+      <c r="D83" t="s">
+        <v>58</v>
+      </c>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" t="s">
+        <v>74</v>
+      </c>
+      <c r="D84" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" t="s">
+        <v>121</v>
+      </c>
+      <c r="D85" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" t="s">
+        <v>74</v>
+      </c>
+      <c r="D86" t="s">
+        <v>30</v>
+      </c>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>99</v>
+      </c>
+      <c r="C87" t="s">
+        <v>74</v>
+      </c>
+      <c r="D87" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" t="s">
+        <v>74</v>
+      </c>
+      <c r="D88" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" t="s">
+        <v>74</v>
+      </c>
+      <c r="D89" t="s">
+        <v>30</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>102</v>
+      </c>
+      <c r="C90" t="s">
+        <v>74</v>
+      </c>
+      <c r="D90" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>103</v>
+      </c>
+      <c r="C91" t="s">
+        <v>74</v>
+      </c>
+      <c r="D91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>104</v>
+      </c>
+      <c r="C92" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>105</v>
+      </c>
+      <c r="C93" t="s">
+        <v>74</v>
+      </c>
+      <c r="D93" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" t="s">
+        <v>123</v>
+      </c>
+      <c r="D94" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>107</v>
+      </c>
+      <c r="C95" t="s">
+        <v>74</v>
+      </c>
+      <c r="D95" t="s">
+        <v>31</v>
+      </c>
+      <c r="F95" s="1"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C96" t="s">
+        <v>74</v>
+      </c>
+      <c r="D96" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C97" t="s">
+        <v>74</v>
+      </c>
+      <c r="D97" t="s">
+        <v>30</v>
+      </c>
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>110</v>
+      </c>
+      <c r="C98" t="s">
+        <v>74</v>
+      </c>
+      <c r="D98" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>111</v>
+      </c>
+      <c r="C99" t="s">
+        <v>74</v>
+      </c>
+      <c r="D99" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" t="s">
+        <v>122</v>
+      </c>
+      <c r="D100" t="s">
+        <v>31</v>
+      </c>
+      <c r="F100" s="1"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>113</v>
+      </c>
+      <c r="C101" t="s">
+        <v>124</v>
+      </c>
+      <c r="D101" t="s">
+        <v>31</v>
+      </c>
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>114</v>
+      </c>
+      <c r="C102" t="s">
+        <v>123</v>
+      </c>
+      <c r="D102" t="s">
+        <v>31</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>115</v>
+      </c>
+      <c r="C103" t="s">
+        <v>125</v>
+      </c>
+      <c r="D103" t="s">
+        <v>31</v>
+      </c>
+      <c r="F103" s="1"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>116</v>
+      </c>
+      <c r="C104" t="s">
+        <v>126</v>
+      </c>
+      <c r="D104" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>117</v>
+      </c>
+      <c r="C105" t="s">
+        <v>74</v>
+      </c>
+      <c r="D105" t="s">
+        <v>30</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>118</v>
+      </c>
+      <c r="C106" t="s">
+        <v>74</v>
+      </c>
+      <c r="D106" t="s">
+        <v>30</v>
+      </c>
+      <c r="E106" t="s">
+        <v>29</v>
+      </c>
+      <c r="F106" s="1"/>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>132</v>
+      </c>
+      <c r="C107" t="s">
+        <v>140</v>
+      </c>
+      <c r="D107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C108" t="s">
+        <v>140</v>
+      </c>
+      <c r="D108" t="s">
+        <v>30</v>
+      </c>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>133</v>
+      </c>
+      <c r="C109" t="s">
+        <v>141</v>
+      </c>
+      <c r="D109" t="s">
+        <v>31</v>
+      </c>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" t="s">
+        <v>140</v>
+      </c>
+      <c r="D110" t="s">
+        <v>30</v>
+      </c>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>134</v>
+      </c>
+      <c r="C111" t="s">
+        <v>140</v>
+      </c>
+      <c r="D111" t="s">
+        <v>30</v>
+      </c>
+      <c r="F111" s="1"/>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>135</v>
+      </c>
+      <c r="C112" t="s">
+        <v>140</v>
+      </c>
+      <c r="D112" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>138</v>
+      </c>
+      <c r="C113" t="s">
+        <v>140</v>
+      </c>
+      <c r="D113" t="s">
+        <v>30</v>
+      </c>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>139</v>
+      </c>
+      <c r="C114" t="s">
+        <v>140</v>
+      </c>
+      <c r="D114" t="s">
+        <v>30</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F114" s="1"/>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>143</v>
+      </c>
+      <c r="C115" t="s">
+        <v>142</v>
+      </c>
+      <c r="D115" t="s">
+        <v>30</v>
+      </c>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>144</v>
+      </c>
+      <c r="C116" t="s">
+        <v>142</v>
+      </c>
+      <c r="D116" t="s">
+        <v>30</v>
+      </c>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>145</v>
+      </c>
+      <c r="C117" t="s">
+        <v>142</v>
+      </c>
+      <c r="D117" t="s">
+        <v>30</v>
+      </c>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>146</v>
+      </c>
+      <c r="C118" t="s">
+        <v>142</v>
+      </c>
+      <c r="D118" t="s">
+        <v>240</v>
+      </c>
+      <c r="F118" s="1"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>158</v>
+      </c>
+      <c r="C119" t="s">
+        <v>142</v>
+      </c>
+      <c r="D119" t="s">
+        <v>30</v>
+      </c>
+      <c r="F119" s="1"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>147</v>
+      </c>
+      <c r="C120" t="s">
+        <v>159</v>
+      </c>
+      <c r="D120" t="s">
+        <v>31</v>
+      </c>
+      <c r="F120" s="1"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>148</v>
+      </c>
+      <c r="C121" t="s">
+        <v>166</v>
+      </c>
+      <c r="D121" t="s">
+        <v>31</v>
+      </c>
+      <c r="F121" s="1"/>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>149</v>
+      </c>
+      <c r="C122" t="s">
+        <v>142</v>
+      </c>
+      <c r="D122" t="s">
+        <v>30</v>
+      </c>
+      <c r="F122" s="1"/>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>160</v>
+      </c>
+      <c r="C123" t="s">
+        <v>161</v>
+      </c>
+      <c r="D123" t="s">
+        <v>31</v>
+      </c>
+      <c r="F123" s="1"/>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>150</v>
+      </c>
+      <c r="C124" t="s">
+        <v>162</v>
+      </c>
+      <c r="D124" t="s">
+        <v>30</v>
+      </c>
+      <c r="F124" s="1"/>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>163</v>
+      </c>
+      <c r="C125" t="s">
+        <v>142</v>
+      </c>
+      <c r="D125" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>164</v>
+      </c>
+      <c r="C126" t="s">
+        <v>142</v>
+      </c>
+      <c r="D126" t="s">
+        <v>30</v>
+      </c>
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>151</v>
+      </c>
+      <c r="C127" t="s">
+        <v>142</v>
+      </c>
+      <c r="D127" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>152</v>
+      </c>
+      <c r="C128" t="s">
+        <v>142</v>
+      </c>
+      <c r="D128" t="s">
+        <v>30</v>
+      </c>
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" t="s">
+        <v>142</v>
+      </c>
+      <c r="D129" t="s">
+        <v>30</v>
+      </c>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>154</v>
+      </c>
+      <c r="C130" t="s">
+        <v>165</v>
+      </c>
+      <c r="D130" t="s">
+        <v>31</v>
+      </c>
+      <c r="F130" s="1"/>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>155</v>
+      </c>
+      <c r="C131" t="s">
+        <v>159</v>
+      </c>
+      <c r="D131" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>156</v>
+      </c>
+      <c r="C132" t="s">
+        <v>142</v>
+      </c>
+      <c r="D132" t="s">
+        <v>30</v>
+      </c>
+      <c r="F132" s="1"/>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>157</v>
+      </c>
+      <c r="C133" t="s">
+        <v>142</v>
+      </c>
+      <c r="D133" t="s">
+        <v>30</v>
+      </c>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>168</v>
+      </c>
+      <c r="C134" t="s">
+        <v>167</v>
+      </c>
+      <c r="D134" t="s">
+        <v>30</v>
+      </c>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>169</v>
+      </c>
+      <c r="C135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D135" t="s">
+        <v>31</v>
+      </c>
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>170</v>
+      </c>
+      <c r="C136" t="s">
+        <v>176</v>
+      </c>
+      <c r="D136" t="s">
+        <v>31</v>
+      </c>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>152</v>
+      </c>
+      <c r="C137" t="s">
+        <v>167</v>
+      </c>
+      <c r="D137" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>171</v>
+      </c>
+      <c r="C138" t="s">
+        <v>167</v>
+      </c>
+      <c r="D138" t="s">
+        <v>30</v>
+      </c>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>172</v>
+      </c>
+      <c r="C139" t="s">
+        <v>167</v>
+      </c>
+      <c r="D139" t="s">
+        <v>30</v>
+      </c>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" t="s">
+        <v>167</v>
+      </c>
+      <c r="D140" t="s">
+        <v>30</v>
+      </c>
+      <c r="E140" t="s">
+        <v>29</v>
+      </c>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>174</v>
+      </c>
+      <c r="C141" t="s">
+        <v>167</v>
+      </c>
+      <c r="D141" t="s">
+        <v>30</v>
+      </c>
+      <c r="E141" t="s">
+        <v>29</v>
+      </c>
+      <c r="F141" s="1"/>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>177</v>
+      </c>
+      <c r="C142" t="s">
+        <v>182</v>
+      </c>
+      <c r="D142" t="s">
+        <v>30</v>
+      </c>
+      <c r="E142" s="1"/>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>178</v>
+      </c>
+      <c r="C143" t="s">
+        <v>182</v>
+      </c>
+      <c r="D143" t="s">
+        <v>30</v>
+      </c>
+      <c r="F143" s="1"/>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>179</v>
+      </c>
+      <c r="C144" t="s">
+        <v>182</v>
+      </c>
+      <c r="D144" t="s">
+        <v>30</v>
+      </c>
+      <c r="F144" s="1"/>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>184</v>
+      </c>
+      <c r="C145" t="s">
+        <v>183</v>
+      </c>
+      <c r="D145" t="s">
+        <v>30</v>
+      </c>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>180</v>
+      </c>
+      <c r="C146" t="s">
+        <v>182</v>
+      </c>
+      <c r="D146" t="s">
+        <v>30</v>
+      </c>
+      <c r="F146" s="1"/>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>181</v>
+      </c>
+      <c r="C147" t="s">
+        <v>182</v>
+      </c>
+      <c r="D147" t="s">
+        <v>30</v>
+      </c>
+      <c r="E147" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>185</v>
+      </c>
+      <c r="C148" t="s">
+        <v>186</v>
+      </c>
+      <c r="D148" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>187</v>
+      </c>
+      <c r="C149" t="s">
+        <v>206</v>
+      </c>
+      <c r="D149" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>188</v>
+      </c>
+      <c r="C150" t="s">
+        <v>206</v>
+      </c>
+      <c r="D150" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>189</v>
+      </c>
+      <c r="C151" t="s">
+        <v>206</v>
+      </c>
+      <c r="D151" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>190</v>
+      </c>
+      <c r="C152" t="s">
+        <v>206</v>
+      </c>
+      <c r="D152" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>191</v>
+      </c>
+      <c r="C153" t="s">
+        <v>207</v>
+      </c>
+      <c r="D153" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>192</v>
+      </c>
+      <c r="C154" t="s">
+        <v>206</v>
+      </c>
+      <c r="D154" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>208</v>
+      </c>
+      <c r="C155" t="s">
+        <v>206</v>
+      </c>
+      <c r="D155" t="s">
+        <v>30</v>
+      </c>
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>193</v>
+      </c>
+      <c r="C156" t="s">
+        <v>206</v>
+      </c>
+      <c r="D156" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>194</v>
+      </c>
+      <c r="C157" t="s">
+        <v>206</v>
+      </c>
+      <c r="D157" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>195</v>
+      </c>
+      <c r="C158" t="s">
+        <v>206</v>
+      </c>
+      <c r="D158" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B159" t="s">
+        <v>196</v>
+      </c>
+      <c r="C159" t="s">
+        <v>209</v>
+      </c>
+      <c r="D159" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B160" t="s">
+        <v>197</v>
+      </c>
+      <c r="C160" t="s">
+        <v>206</v>
+      </c>
+      <c r="D160" t="s">
+        <v>30</v>
+      </c>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B161" t="s">
+        <v>198</v>
+      </c>
+      <c r="C161" t="s">
+        <v>206</v>
+      </c>
+      <c r="D161" t="s">
+        <v>30</v>
+      </c>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B162" t="s">
+        <v>199</v>
+      </c>
+      <c r="C162" t="s">
+        <v>206</v>
+      </c>
+      <c r="D162" t="s">
+        <v>30</v>
+      </c>
+      <c r="F162" s="1"/>
+    </row>
+    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B163" t="s">
+        <v>200</v>
+      </c>
+      <c r="C163" t="s">
+        <v>206</v>
+      </c>
+      <c r="D163" t="s">
+        <v>30</v>
+      </c>
+      <c r="F163" s="1"/>
+    </row>
+    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B164" t="s">
+        <v>201</v>
+      </c>
+      <c r="C164" t="s">
+        <v>206</v>
+      </c>
+      <c r="D164" t="s">
+        <v>30</v>
+      </c>
+      <c r="F164" s="1"/>
+    </row>
+    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B165" t="s">
+        <v>202</v>
+      </c>
+      <c r="C165" t="s">
+        <v>206</v>
+      </c>
+      <c r="D165" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B166" t="s">
+        <v>203</v>
+      </c>
+      <c r="C166" t="s">
+        <v>206</v>
+      </c>
+      <c r="D166" t="s">
+        <v>30</v>
+      </c>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+    </row>
+    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B167" t="s">
+        <v>204</v>
+      </c>
+      <c r="C167" t="s">
+        <v>206</v>
+      </c>
+      <c r="D167" t="s">
+        <v>31</v>
+      </c>
+      <c r="F167" s="1"/>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B168" t="s">
+        <v>205</v>
+      </c>
+      <c r="C168" t="s">
+        <v>206</v>
+      </c>
+      <c r="D168" t="s">
+        <v>30</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F168" s="1"/>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B169" t="s">
+        <v>211</v>
+      </c>
+      <c r="C169" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>212</v>
+      </c>
+      <c r="C170" t="s">
+        <v>239</v>
+      </c>
+      <c r="D170" t="s">
+        <v>31</v>
+      </c>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B171" t="s">
+        <v>213</v>
+      </c>
+      <c r="C171" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B172" t="s">
+        <v>214</v>
+      </c>
+      <c r="C172" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>215</v>
+      </c>
+      <c r="C173" t="s">
+        <v>210</v>
+      </c>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B174" t="s">
+        <v>216</v>
+      </c>
+      <c r="C174" t="s">
+        <v>242</v>
+      </c>
+      <c r="D174" t="s">
+        <v>31</v>
+      </c>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>231</v>
+      </c>
+      <c r="C175" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B176" t="s">
+        <v>217</v>
+      </c>
+      <c r="C176" t="s">
+        <v>238</v>
+      </c>
+      <c r="D176" t="s">
+        <v>31</v>
+      </c>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B177" t="s">
+        <v>232</v>
+      </c>
+      <c r="C177" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>218</v>
+      </c>
+      <c r="C178" t="s">
+        <v>210</v>
+      </c>
+      <c r="D178" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B179" t="s">
+        <v>219</v>
+      </c>
+      <c r="C179" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B180" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B181" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B182" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B183" t="s">
+        <v>222</v>
+      </c>
+      <c r="F183" s="1"/>
+    </row>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B185" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="186" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B186" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B187" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B188" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B189" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="190" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B190" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="191" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B191" t="s">
+        <v>237</v>
+      </c>
+      <c r="E191" s="1"/>
+      <c r="F191" s="1"/>
+    </row>
+    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B192" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B193" t="s">
+        <v>228</v>
+      </c>
+      <c r="F193" s="1"/>
+    </row>
+    <row r="194" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="195" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="198" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F198" s="1"/>
+    </row>
+    <row r="201" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E201" s="1"/>
+    </row>
+    <row r="203" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E203" s="1"/>
+    </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F204" s="1"/>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F205" s="1"/>
+    </row>
+    <row r="207" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E207" s="1"/>
+    </row>
+    <row r="209" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E209" s="1"/>
+    </row>
+    <row r="211" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F211" s="1"/>
+    </row>
+    <row r="214" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E214" s="1"/>
+    </row>
+    <row r="215" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F215" s="1"/>
+    </row>
+    <row r="217" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+    </row>
+    <row r="220" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E220" s="1"/>
+      <c r="F220" s="1"/>
+    </row>
+    <row r="227" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F227" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>